<commit_message>
updated input file, queries, bento profile, keyword etc
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_Filter_Diagnosis-Adenocarcinoma.xlsx
+++ b/InputFiles/TC01_Bento_Filter_Diagnosis-Adenocarcinoma.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E544BD03-2C92-4D88-9973-E836811E3C7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1F4881-1D4A-469F-A382-2E1FEAD7C4B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="10" windowWidth="19140" windowHeight="10190" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="60" yWindow="10" windowWidth="19140" windowHeight="10190" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>WebExcel</t>
   </si>
@@ -55,6 +55,40 @@
   </si>
   <si>
     <t>TC01_Bento_Filter_Diagnosis-Adenocarcinoma_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>SamplesTab</t>
+  </si>
+  <si>
+    <t>FilesTab</t>
+  </si>
+  <si>
+    <t>MATCH (ss:study_subject)
+WITH COLLECT(ss.study_subject_id) AS all_subjects
+MATCH (samp:sample)
+MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
+MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
+MATCH (samp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
+MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
+MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
+WHERE ss.disease_subtype IN ["Adenocarcinoma"] and sf.grouped_recurrence_score IN ["0-5"]  and d.tumor_size_group In ["Not Reported"]
+WITH
+    distinct lp,
+    toInteger(split(ss.study_subject_id,'-')[2]) AS subject_id_num,
+    collect(distinct f.file_id) AS files,
+    samp, ss, s, p, all_subjects
+RETURN
+ samp.sample_id AS `Sample ID`,
+            ss.study_subject_id AS `Case ID`,
+            p.program_acronym AS `Program Code`,
+            s.study_acronym AS `Arm`,
+            ss.disease_subtype AS `Diagnosis`,
+            samp.tissue_type AS `Tissue Type`,
+            samp.composition AS `Tissue Composition`,
+            samp.sample_anatomic_site AS `Sample Anatomic Site`,
+            samp.method_of_sample_procurement AS `Sample Procurement Method`,
+            lp.test_name as Platform</t>
   </si>
   <si>
     <t>MATCH (ss:study_subject)
@@ -65,7 +99,7 @@
 MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
 MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
 MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
-WHERE ss.disease_subtype IN ["Adenocarcinoma"] and d.tumor_grade In ["Intermediate Grade"]
+ WHERE ss.disease_subtype IN ["Adenocarcinoma"] and sf.grouped_recurrence_score IN ["0-5"] and d.tumor_size_group In ["Not Reported"]
 return ss.study_subject_id as `Case ID`,
        p.program_acronym as `Program Code`,
         p.program_id as Program_ID,
@@ -75,7 +109,29 @@
        d.tumor_size_group AS `tumor_size`,
        d.er_status AS `ER Status`,
        d.pr_status AS `PR Status`,
-       demo.age_at_index AS `Age (years)`</t>
+       demo.age_at_index AS `Age (years)`,
+demo.survival_time AS `Survival (days)`</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)
+MATCH (f)-[:file_of_sample]-&gt;(samp)
+MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
+MATCH (ss)-[:study_subject_of_study]-&gt;(s)
+MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
+MATCH (s)-[:study_of_program]-&gt;(p)
+MATCH (d)-[:diagnosis_of_study_subject]-&gt;(ss)
+MATCH (tp)-[:tp_of_diagnosis]-&gt;(d)
+ WHERE ss.disease_subtype IN ["Adenocarcinoma"] and sf.grouped_recurrence_score IN ["0-5"] and d.tumor_size_group In ["Not Reported"]
+RETURN  f.file_name AS `File Name`,
+    head(labels(samp)) AS `Association`,
+    f.file_description AS `Description`,
+    f.file_format AS `File Format`,
+    f.file_size AS `Size`,
+    p.program_acronym AS `Program Code`,
+    s.study_acronym AS `Arm`,
+    ss.study_subject_id AS `Case ID`,
+    samp.sample_id AS `Sample ID`,
+    ss.disease_subtype as `Diagnosis`</t>
   </si>
   <si>
     <t>MATCH (ss:study_subject)
@@ -464,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -496,20 +552,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
bento localfind upload csv and txt completed
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Bento_Filter_Diagnosis-Adenocarcinoma.xlsx
+++ b/InputFiles/TC01_Bento_Filter_Diagnosis-Adenocarcinoma.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7255A522-9FB9-424B-8E22-B9361C17DBE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4576AB-FD1D-4FDB-B3D8-B4E6CE8E0E46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="9800" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>